<commit_message>
Revert "minimum number of steps required to sort an array"
This reverts commit d0eae406c75c1642f541b9c1cfa1059aa209fe7c.
</commit_message>
<xml_diff>
--- a/AlgoDs.xlsx
+++ b/AlgoDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUN\Desktop\TopicsAlGoDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A0699B-23AD-4BB0-993C-E7C678C10B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDB12C0-F318-4FA5-AED4-35E71224EB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{030A3091-96FF-4395-AB41-93B5B5BF05AB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>List of algorithms and datastructures</t>
   </si>
@@ -93,12 +93,6 @@
   </si>
   <si>
     <t>(19)Self Balancing trees(Avl tree And red black tree)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">( 20)quick  sort (randomized sort, finding median in O(N) time)       </t>
-  </si>
-  <si>
-    <t>(21)search one pair linearly and swap them to sort the array.</t>
   </si>
 </sst>
 </file>
@@ -459,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625C2889-4FA1-40F1-BECA-2E024767759A}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,13 +562,8 @@
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
+      <c r="A21">
+        <v>-20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>